<commit_message>
update T1C Pool / fix minor bug / add preload in save update button.
</commit_message>
<xml_diff>
--- a/Budget/Template_BudgetFGVPISB.xlsx
+++ b/Budget/Template_BudgetFGVPISB.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>NO</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Chalok</t>
+  </si>
+  <si>
+    <t>YEAR</t>
   </si>
 </sst>
 </file>
@@ -167,10 +170,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -486,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +502,7 @@
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,8 +551,11 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -597,8 +604,11 @@
       <c r="P2" s="2">
         <v>125547.5</v>
       </c>
+      <c r="Q2" s="3">
+        <v>2025</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -647,8 +657,11 @@
       <c r="P3" s="2">
         <v>95260</v>
       </c>
+      <c r="Q3" s="3">
+        <v>2025</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -697,8 +710,11 @@
       <c r="P4" s="2">
         <v>132228</v>
       </c>
+      <c r="Q4" s="3">
+        <v>2025</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -747,8 +763,11 @@
       <c r="P5" s="2">
         <v>120555</v>
       </c>
+      <c r="Q5" s="3">
+        <v>2025</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -797,8 +816,11 @@
       <c r="P6" s="2">
         <v>82695</v>
       </c>
+      <c r="Q6" s="3">
+        <v>2025</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -847,8 +869,11 @@
       <c r="P7" s="2">
         <v>104600</v>
       </c>
+      <c r="Q7" s="3">
+        <v>2025</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -897,8 +922,11 @@
       <c r="P8" s="2">
         <v>148482.5</v>
       </c>
+      <c r="Q8" s="3">
+        <v>2025</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -947,8 +975,11 @@
       <c r="P9" s="2">
         <v>92837.5</v>
       </c>
+      <c r="Q9" s="3">
+        <v>2025</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -996,6 +1027,9 @@
       </c>
       <c r="P10" s="2">
         <v>108200</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>2025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>